<commit_message>
finished event information tab
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="193" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="207" uniqueCount="156">
   <si>
     <t>Club Event Report Form for</t>
   </si>
@@ -1686,10 +1686,31 @@
     <t>Board Meeting #3</t>
   </si>
   <si>
-    <t>testing!</t>
+    <t>editCell test</t>
   </si>
   <si>
-    <t>s</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -8217,10 +8238,10 @@
       <c r="D24" s="214"/>
       <c r="E24" s="220"/>
       <c r="F24" s="35" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="H24" s="220"/>
       <c r="I24" s="210" t="s">
@@ -8254,7 +8275,9 @@
       <c r="F25" s="63"/>
       <c r="G25" s="63"/>
       <c r="H25" s="220"/>
-      <c r="I25" s="215"/>
+      <c r="I25" s="215" t="s">
+        <v>153</v>
+      </c>
       <c r="J25" s="213"/>
       <c r="K25" s="213"/>
       <c r="L25" s="213"/>
@@ -8309,7 +8332,9 @@
     </row>
     <row r="27" ht="16.25" customHeight="true" x14ac:dyDescent="0.2">
       <c r="A27" s="249"/>
-      <c r="B27" s="216"/>
+      <c r="B27" s="216" t="s">
+        <v>149</v>
+      </c>
       <c r="C27" s="217"/>
       <c r="D27" s="218"/>
       <c r="E27" s="220"/>
@@ -8383,7 +8408,9 @@
       </c>
       <c r="G29" s="82"/>
       <c r="H29" s="220"/>
-      <c r="I29" s="215"/>
+      <c r="I29" s="215" t="s">
+        <v>154</v>
+      </c>
       <c r="J29" s="213"/>
       <c r="K29" s="213"/>
       <c r="L29" s="213"/>
@@ -8405,7 +8432,9 @@
     </row>
     <row r="30" ht="16.25" customHeight="true" x14ac:dyDescent="0.2">
       <c r="A30" s="249"/>
-      <c r="B30" s="286"/>
+      <c r="B30" s="286" t="s">
+        <v>150</v>
+      </c>
       <c r="C30" s="287"/>
       <c r="D30" s="288"/>
       <c r="E30" s="220"/>
@@ -8630,7 +8659,9 @@
       <c r="D37" s="231"/>
       <c r="E37" s="231"/>
       <c r="F37" s="232"/>
-      <c r="G37" s="32"/>
+      <c r="G37" s="32" t="s">
+        <v>155</v>
+      </c>
       <c r="H37" s="229"/>
       <c r="I37" s="229"/>
       <c r="J37" s="200" t="s">
@@ -8650,7 +8681,9 @@
       <c r="V37" s="200"/>
       <c r="W37" s="200"/>
       <c r="X37" s="200"/>
-      <c r="Y37" s="201"/>
+      <c r="Y37" s="201" t="s">
+        <v>155</v>
+      </c>
       <c r="Z37" s="202"/>
       <c r="AA37" s="203"/>
     </row>
@@ -8696,7 +8729,9 @@
       <c r="D39" s="231"/>
       <c r="E39" s="231"/>
       <c r="F39" s="232"/>
-      <c r="G39" s="60"/>
+      <c r="G39" s="60" t="s">
+        <v>155</v>
+      </c>
       <c r="H39" s="229"/>
       <c r="I39" s="229"/>
       <c r="J39" s="253" t="s">
@@ -8749,7 +8784,9 @@
       <c r="V40" s="256"/>
       <c r="W40" s="256"/>
       <c r="X40" s="256"/>
-      <c r="Y40" s="201"/>
+      <c r="Y40" s="201" t="s">
+        <v>155</v>
+      </c>
       <c r="Z40" s="202"/>
       <c r="AA40" s="203"/>
     </row>
@@ -8795,7 +8832,9 @@
       <c r="D42" s="258"/>
       <c r="E42" s="258"/>
       <c r="F42" s="258"/>
-      <c r="G42" s="60"/>
+      <c r="G42" s="60" t="s">
+        <v>155</v>
+      </c>
       <c r="H42" s="229"/>
       <c r="I42" s="229"/>
       <c r="J42" s="200" t="s">
@@ -8846,7 +8885,9 @@
       <c r="V43" s="200"/>
       <c r="W43" s="200"/>
       <c r="X43" s="200"/>
-      <c r="Y43" s="201"/>
+      <c r="Y43" s="201" t="s">
+        <v>155</v>
+      </c>
       <c r="Z43" s="202"/>
       <c r="AA43" s="203"/>
     </row>
@@ -8914,7 +8955,9 @@
       <c r="V45" s="200"/>
       <c r="W45" s="200"/>
       <c r="X45" s="200"/>
-      <c r="Y45" s="201"/>
+      <c r="Y45" s="201" t="s">
+        <v>155</v>
+      </c>
       <c r="Z45" s="202"/>
       <c r="AA45" s="203"/>
     </row>
@@ -8945,7 +8988,9 @@
       <c r="V46" s="200"/>
       <c r="W46" s="200"/>
       <c r="X46" s="200"/>
-      <c r="Y46" s="201"/>
+      <c r="Y46" s="201" t="s">
+        <v>155</v>
+      </c>
       <c r="Z46" s="202"/>
       <c r="AA46" s="203"/>
     </row>

</xml_diff>

<commit_message>
add new part to GUI
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="207" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="202" uniqueCount="150">
   <si>
     <t>Club Event Report Form for</t>
   </si>
@@ -1689,25 +1689,7 @@
     <t>editCell test</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
+    <t/>
   </si>
   <si>
     <t>x</t>
@@ -8238,10 +8220,10 @@
       <c r="D24" s="214"/>
       <c r="E24" s="220"/>
       <c r="F24" s="35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H24" s="220"/>
       <c r="I24" s="210" t="s">
@@ -8276,7 +8258,7 @@
       <c r="G25" s="63"/>
       <c r="H25" s="220"/>
       <c r="I25" s="215" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J25" s="213"/>
       <c r="K25" s="213"/>
@@ -8333,7 +8315,7 @@
     <row r="27" ht="16.25" customHeight="true" x14ac:dyDescent="0.2">
       <c r="A27" s="249"/>
       <c r="B27" s="216" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C27" s="217"/>
       <c r="D27" s="218"/>
@@ -8409,7 +8391,7 @@
       <c r="G29" s="82"/>
       <c r="H29" s="220"/>
       <c r="I29" s="215" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J29" s="213"/>
       <c r="K29" s="213"/>
@@ -8433,7 +8415,7 @@
     <row r="30" ht="16.25" customHeight="true" x14ac:dyDescent="0.2">
       <c r="A30" s="249"/>
       <c r="B30" s="286" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C30" s="287"/>
       <c r="D30" s="288"/>
@@ -8660,7 +8642,7 @@
       <c r="E37" s="231"/>
       <c r="F37" s="232"/>
       <c r="G37" s="32" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H37" s="229"/>
       <c r="I37" s="229"/>
@@ -8681,9 +8663,7 @@
       <c r="V37" s="200"/>
       <c r="W37" s="200"/>
       <c r="X37" s="200"/>
-      <c r="Y37" s="201" t="s">
-        <v>155</v>
-      </c>
+      <c r="Y37" s="201"/>
       <c r="Z37" s="202"/>
       <c r="AA37" s="203"/>
     </row>
@@ -8716,7 +8696,9 @@
       <c r="V38" s="200"/>
       <c r="W38" s="200"/>
       <c r="X38" s="200"/>
-      <c r="Y38" s="201"/>
+      <c r="Y38" s="201" t="s">
+        <v>149</v>
+      </c>
       <c r="Z38" s="202"/>
       <c r="AA38" s="203"/>
     </row>
@@ -8729,9 +8711,7 @@
       <c r="D39" s="231"/>
       <c r="E39" s="231"/>
       <c r="F39" s="232"/>
-      <c r="G39" s="60" t="s">
-        <v>155</v>
-      </c>
+      <c r="G39" s="60"/>
       <c r="H39" s="229"/>
       <c r="I39" s="229"/>
       <c r="J39" s="253" t="s">
@@ -8784,9 +8764,7 @@
       <c r="V40" s="256"/>
       <c r="W40" s="256"/>
       <c r="X40" s="256"/>
-      <c r="Y40" s="201" t="s">
-        <v>155</v>
-      </c>
+      <c r="Y40" s="201"/>
       <c r="Z40" s="202"/>
       <c r="AA40" s="203"/>
     </row>
@@ -8832,9 +8810,7 @@
       <c r="D42" s="258"/>
       <c r="E42" s="258"/>
       <c r="F42" s="258"/>
-      <c r="G42" s="60" t="s">
-        <v>155</v>
-      </c>
+      <c r="G42" s="60"/>
       <c r="H42" s="229"/>
       <c r="I42" s="229"/>
       <c r="J42" s="200" t="s">
@@ -8886,7 +8862,7 @@
       <c r="W43" s="200"/>
       <c r="X43" s="200"/>
       <c r="Y43" s="201" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="Z43" s="202"/>
       <c r="AA43" s="203"/>
@@ -8955,9 +8931,7 @@
       <c r="V45" s="200"/>
       <c r="W45" s="200"/>
       <c r="X45" s="200"/>
-      <c r="Y45" s="201" t="s">
-        <v>155</v>
-      </c>
+      <c r="Y45" s="201"/>
       <c r="Z45" s="202"/>
       <c r="AA45" s="203"/>
     </row>
@@ -8988,9 +8962,7 @@
       <c r="V46" s="200"/>
       <c r="W46" s="200"/>
       <c r="X46" s="200"/>
-      <c r="Y46" s="201" t="s">
-        <v>155</v>
-      </c>
+      <c r="Y46" s="201"/>
       <c r="Z46" s="202"/>
       <c r="AA46" s="203"/>
     </row>

</xml_diff>

<commit_message>
working on second gui
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="202" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="207" uniqueCount="151">
   <si>
     <t>Club Event Report Form for</t>
   </si>
@@ -1692,6 +1692,9 @@
     <t/>
   </si>
   <si>
+    <t>d</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
 </sst>
@@ -8220,7 +8223,7 @@
       <c r="D24" s="214"/>
       <c r="E24" s="220"/>
       <c r="F24" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G24" s="36" t="s">
         <v>148</v>
@@ -8315,7 +8318,7 @@
     <row r="27" ht="16.25" customHeight="true" x14ac:dyDescent="0.2">
       <c r="A27" s="249"/>
       <c r="B27" s="216" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C27" s="217"/>
       <c r="D27" s="218"/>
@@ -8391,7 +8394,7 @@
       <c r="G29" s="82"/>
       <c r="H29" s="220"/>
       <c r="I29" s="215" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J29" s="213"/>
       <c r="K29" s="213"/>
@@ -8415,7 +8418,7 @@
     <row r="30" ht="16.25" customHeight="true" x14ac:dyDescent="0.2">
       <c r="A30" s="249"/>
       <c r="B30" s="286" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C30" s="287"/>
       <c r="D30" s="288"/>
@@ -8641,9 +8644,7 @@
       <c r="D37" s="231"/>
       <c r="E37" s="231"/>
       <c r="F37" s="232"/>
-      <c r="G37" s="32" t="s">
-        <v>149</v>
-      </c>
+      <c r="G37" s="32"/>
       <c r="H37" s="229"/>
       <c r="I37" s="229"/>
       <c r="J37" s="200" t="s">
@@ -8676,7 +8677,9 @@
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
       <c r="F38" s="30"/>
-      <c r="G38" s="60"/>
+      <c r="G38" s="60" t="s">
+        <v>150</v>
+      </c>
       <c r="H38" s="229"/>
       <c r="I38" s="229"/>
       <c r="J38" s="200" t="s">
@@ -8696,9 +8699,7 @@
       <c r="V38" s="200"/>
       <c r="W38" s="200"/>
       <c r="X38" s="200"/>
-      <c r="Y38" s="201" t="s">
-        <v>149</v>
-      </c>
+      <c r="Y38" s="201"/>
       <c r="Z38" s="202"/>
       <c r="AA38" s="203"/>
     </row>
@@ -8777,7 +8778,9 @@
       <c r="D41" s="241"/>
       <c r="E41" s="241"/>
       <c r="F41" s="242"/>
-      <c r="G41" s="60"/>
+      <c r="G41" s="60" t="s">
+        <v>150</v>
+      </c>
       <c r="H41" s="229"/>
       <c r="I41" s="229"/>
       <c r="J41" s="200" t="s">
@@ -8797,7 +8800,9 @@
       <c r="V41" s="200"/>
       <c r="W41" s="200"/>
       <c r="X41" s="200"/>
-      <c r="Y41" s="201"/>
+      <c r="Y41" s="201" t="s">
+        <v>150</v>
+      </c>
       <c r="Z41" s="202"/>
       <c r="AA41" s="203"/>
     </row>
@@ -8830,7 +8835,9 @@
       <c r="V42" s="200"/>
       <c r="W42" s="200"/>
       <c r="X42" s="200"/>
-      <c r="Y42" s="201"/>
+      <c r="Y42" s="201" t="s">
+        <v>150</v>
+      </c>
       <c r="Z42" s="202"/>
       <c r="AA42" s="203"/>
     </row>
@@ -8862,7 +8869,7 @@
       <c r="W43" s="200"/>
       <c r="X43" s="200"/>
       <c r="Y43" s="201" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Z43" s="202"/>
       <c r="AA43" s="203"/>
@@ -8911,7 +8918,9 @@
       <c r="D45" s="239"/>
       <c r="E45" s="239"/>
       <c r="F45" s="239"/>
-      <c r="G45" s="61"/>
+      <c r="G45" s="61" t="s">
+        <v>150</v>
+      </c>
       <c r="H45" s="229"/>
       <c r="I45" s="229"/>
       <c r="J45" s="200" t="s">
@@ -8931,7 +8940,9 @@
       <c r="V45" s="200"/>
       <c r="W45" s="200"/>
       <c r="X45" s="200"/>
-      <c r="Y45" s="201"/>
+      <c r="Y45" s="201" t="s">
+        <v>150</v>
+      </c>
       <c r="Z45" s="202"/>
       <c r="AA45" s="203"/>
     </row>
@@ -9037,7 +9048,9 @@
       <c r="D49" s="233"/>
       <c r="E49" s="233"/>
       <c r="F49" s="233"/>
-      <c r="G49" s="61"/>
+      <c r="G49" s="61" t="s">
+        <v>150</v>
+      </c>
       <c r="H49" s="229"/>
       <c r="I49" s="228"/>
       <c r="J49" s="229"/>

</xml_diff>

<commit_message>
added helper classes, working on attendees getting their hours
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="165">
   <si>
     <r>
       <rPr>
@@ -1207,22 +1207,22 @@
     <t>editCell test</t>
   </si>
   <si>
-    <t>Bear Garden Social</t>
+    <t>dd</t>
   </si>
   <si>
-    <t>Jan Daguio</t>
+    <t>ddddddd</t>
   </si>
   <si>
-    <t>01/27/2023</t>
+    <t>ddddd</t>
+  </si>
+  <si>
+    <t>3:00</t>
   </si>
   <si>
     <t>3:00 - 5:00</t>
   </si>
   <si>
-    <t>UC San Diego Town Square</t>
-  </si>
-  <si>
-    <t>Jan Daguio (805) 867-3165</t>
+    <t>dddd</t>
   </si>
   <si>
     <t>Carandang</t>
@@ -7631,12 +7631,12 @@
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="117" t="str">
         <f>F24</f>
-        <v>01/27/2023</v>
+        <v>ddddd</v>
       </c>
       <c r="B18" s="75"/>
       <c r="C18" s="93" t="str">
         <f>B24</f>
-        <v>Bear Garden Social</v>
+        <v>dd</v>
       </c>
       <c r="D18" s="74"/>
       <c r="E18" s="75"/>
@@ -7666,7 +7666,7 @@
       </c>
       <c r="L18" s="8" t="str">
         <f>IF(ISBLANK(G39),"",G39)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="M18" s="8" t="str">
         <f>IF(ISBLANK(G40),"",G40)</f>
@@ -7678,15 +7678,15 @@
       </c>
       <c r="O18" s="8" t="str">
         <f>IF(ISBLANK(G42),"",G42)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="P18" s="8" t="str">
         <f>IF(ISBLANK(G45),"",G45)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="Q18" s="8" t="str">
         <f>IF(ISBLANK(G49), "", G49)</f>
-        <v>x</v>
+        <v/>
       </c>
       <c r="R18" s="8" t="str">
         <f>IF(ISBLANK(Y37), "", Y37)</f>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="S18" s="8" t="str">
         <f>IF(ISBLANK(Y38), "", Y38)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="T18" s="8" t="str">
         <f>IF(ISBLANK(Y39), "", Y39)</f>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="V18" s="8" t="str">
         <f>IF(ISBLANK(Y41), "", Y41)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="W18" s="8" t="str">
         <f>IF(ISBLANK(Y42), "", Y42)</f>
@@ -7726,7 +7726,7 @@
       </c>
       <c r="AA18" s="9" t="str">
         <f>IF(ISBLANK(Y46), "", Y46)</f>
-        <v>x</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7892,7 +7892,7 @@
         <v>147</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H24" s="98"/>
       <c r="I24" s="94" t="s">
@@ -7927,7 +7927,7 @@
       <c r="G25" s="49"/>
       <c r="H25" s="98"/>
       <c r="I25" s="88" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J25" s="74"/>
       <c r="K25" s="74"/>
@@ -8363,7 +8363,9 @@
       <c r="V38" s="74"/>
       <c r="W38" s="74"/>
       <c r="X38" s="75"/>
-      <c r="Y38" s="88"/>
+      <c r="Y38" s="88" t="s">
+        <v>101</v>
+      </c>
       <c r="Z38" s="74"/>
       <c r="AA38" s="75"/>
     </row>
@@ -8376,7 +8378,9 @@
       <c r="D39" s="74"/>
       <c r="E39" s="74"/>
       <c r="F39" s="75"/>
-      <c r="G39" s="15"/>
+      <c r="G39" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="H39" s="113"/>
       <c r="I39" s="114"/>
       <c r="J39" s="115" t="s">
@@ -8462,7 +8466,9 @@
       <c r="V41" s="74"/>
       <c r="W41" s="74"/>
       <c r="X41" s="75"/>
-      <c r="Y41" s="88"/>
+      <c r="Y41" s="88" t="s">
+        <v>101</v>
+      </c>
       <c r="Z41" s="74"/>
       <c r="AA41" s="75"/>
     </row>
@@ -8475,7 +8481,9 @@
       <c r="D42" s="74"/>
       <c r="E42" s="74"/>
       <c r="F42" s="75"/>
-      <c r="G42" s="15"/>
+      <c r="G42" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="H42" s="113"/>
       <c r="I42" s="114"/>
       <c r="J42" s="115" t="s">
@@ -8574,7 +8582,9 @@
       <c r="D45" s="74"/>
       <c r="E45" s="74"/>
       <c r="F45" s="75"/>
-      <c r="G45" s="15"/>
+      <c r="G45" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="H45" s="113"/>
       <c r="I45" s="114"/>
       <c r="J45" s="115" t="s">
@@ -8625,9 +8635,7 @@
       <c r="V46" s="74"/>
       <c r="W46" s="74"/>
       <c r="X46" s="75"/>
-      <c r="Y46" s="88" t="s">
-        <v>101</v>
-      </c>
+      <c r="Y46" s="88"/>
       <c r="Z46" s="74"/>
       <c r="AA46" s="75"/>
     </row>
@@ -8702,9 +8710,7 @@
       <c r="D49" s="74"/>
       <c r="E49" s="74"/>
       <c r="F49" s="75"/>
-      <c r="G49" s="15" t="s">
-        <v>101</v>
-      </c>
+      <c r="G49" s="15"/>
       <c r="H49" s="113"/>
       <c r="I49" s="114"/>
       <c r="J49" s="52"/>

</xml_diff>

<commit_message>
Updated maven and java to JDK 21. Fixed pom.xml
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
   <si>
     <r>
       <rPr>
@@ -1205,33 +1205,6 @@
   </si>
   <si>
     <t>editCell test</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve"> - </t>
-  </si>
-  <si>
-    <t>Hwei</t>
-  </si>
-  <si>
-    <t>Lux</t>
-  </si>
-  <si>
-    <t>Seraphine</t>
-  </si>
-  <si>
-    <t>Sona</t>
-  </si>
-  <si>
-    <t>Samira</t>
-  </si>
-  <si>
-    <t>Nautilus</t>
   </si>
 </sst>
 </file>
@@ -7596,32 +7569,32 @@
       </c>
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="117" t="str">
+      <c r="A18" s="117">
         <f>F24</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B18" s="75"/>
-      <c r="C18" s="93" t="str">
+      <c r="C18" s="93">
         <f>B24</f>
-        <v>e</v>
+        <v>0</v>
       </c>
       <c r="D18" s="74"/>
       <c r="E18" s="75"/>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="7">
         <f>Attendance!A8</f>
-        <v>3.0</v>
+        <v>0</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G18" s="7">
         <f>IF(ISBLANK(Attendance!D8), "", Attendance!D8)</f>
-        <v>4.6</v>
+        <v>0</v>
       </c>
-      <c r="H18" s="7" t="n">
+      <c r="H18" s="7">
         <f>IF(ISBLANK(Attendance!F8), "", Attendance!F8)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="7">
         <f>IF(ISBLANK(Attendance!G8), "", Attendance!G8)</f>
-        <v>4.4</v>
+        <v>0</v>
       </c>
       <c r="J18" s="8" t="str">
         <f>IF(ISBLANK(G37),"",G37)</f>
@@ -7637,15 +7610,15 @@
       </c>
       <c r="M18" s="8" t="str">
         <f>IF(ISBLANK(G40),"",G40)</f>
-        <v>x</v>
+        <v/>
       </c>
       <c r="N18" s="8" t="str">
         <f>IF(ISBLANK(G41),"",G41)</f>
-        <v>x</v>
+        <v/>
       </c>
       <c r="O18" s="8" t="str">
         <f>IF(ISBLANK(G42),"",G42)</f>
-        <v>x</v>
+        <v/>
       </c>
       <c r="P18" s="8" t="str">
         <f>IF(ISBLANK(G45),"",G45)</f>
@@ -7677,7 +7650,7 @@
       </c>
       <c r="W18" s="8" t="str">
         <f>IF(ISBLANK(Y42), "", Y42)</f>
-        <v>x</v>
+        <v/>
       </c>
       <c r="X18" s="8" t="str">
         <f>IF(ISBLANK(Y43), "", Y43)</f>
@@ -7685,7 +7658,7 @@
       </c>
       <c r="Y18" s="8" t="str">
         <f>IF(ISBLANK(Y44), "", Y44)</f>
-        <v>x</v>
+        <v/>
       </c>
       <c r="Z18" s="8" t="str">
         <f>IF(ISBLANK(Y45), "", Y45)</f>
@@ -7850,17 +7823,13 @@
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="101"/>
       <c r="B24" s="88" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" s="74"/>
       <c r="D24" s="75"/>
       <c r="E24" s="98"/>
-      <c r="F24" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>147</v>
-      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="98"/>
       <c r="I24" s="94" t="s">
         <v>71</v>
@@ -7894,7 +7863,7 @@
       <c r="G25" s="49"/>
       <c r="H25" s="98"/>
       <c r="I25" s="88" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="J25" s="74"/>
       <c r="K25" s="74"/>
@@ -7950,15 +7919,13 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="101"/>
-      <c r="B27" s="88" t="s">
-        <v>146</v>
-      </c>
+      <c r="B27" s="88"/>
       <c r="C27" s="74"/>
       <c r="D27" s="75"/>
       <c r="E27" s="98"/>
-      <c r="F27" s="99" t="n">
+      <c r="F27" s="99">
         <f>'Driving Info'!M13</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G27" s="75"/>
       <c r="H27" s="98"/>
@@ -8026,9 +7993,7 @@
       </c>
       <c r="G29" s="75"/>
       <c r="H29" s="98"/>
-      <c r="I29" s="88" t="s">
-        <v>146</v>
-      </c>
+      <c r="I29" s="88"/>
       <c r="J29" s="74"/>
       <c r="K29" s="74"/>
       <c r="L29" s="74"/>
@@ -8050,15 +8015,13 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="101"/>
-      <c r="B30" s="102" t="s">
-        <v>146</v>
-      </c>
+      <c r="B30" s="102"/>
       <c r="C30" s="74"/>
       <c r="D30" s="75"/>
       <c r="E30" s="98"/>
-      <c r="F30" s="118" t="n">
+      <c r="F30" s="118">
         <f>Fundraising!M13</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G30" s="75"/>
       <c r="H30" s="98"/>
@@ -8376,9 +8339,7 @@
       <c r="D40" s="74"/>
       <c r="E40" s="74"/>
       <c r="F40" s="75"/>
-      <c r="G40" s="15" t="s">
-        <v>101</v>
-      </c>
+      <c r="G40" s="15"/>
       <c r="H40" s="113"/>
       <c r="I40" s="114"/>
       <c r="J40" s="115" t="s">
@@ -8411,9 +8372,7 @@
       <c r="D41" s="74"/>
       <c r="E41" s="74"/>
       <c r="F41" s="75"/>
-      <c r="G41" s="15" t="s">
-        <v>101</v>
-      </c>
+      <c r="G41" s="15"/>
       <c r="H41" s="113"/>
       <c r="I41" s="114"/>
       <c r="J41" s="115" t="s">
@@ -8446,9 +8405,7 @@
       <c r="D42" s="74"/>
       <c r="E42" s="74"/>
       <c r="F42" s="75"/>
-      <c r="G42" s="15" t="s">
-        <v>101</v>
-      </c>
+      <c r="G42" s="15"/>
       <c r="H42" s="113"/>
       <c r="I42" s="114"/>
       <c r="J42" s="115" t="s">
@@ -8468,9 +8425,7 @@
       <c r="V42" s="74"/>
       <c r="W42" s="74"/>
       <c r="X42" s="75"/>
-      <c r="Y42" s="88" t="s">
-        <v>101</v>
-      </c>
+      <c r="Y42" s="88"/>
       <c r="Z42" s="74"/>
       <c r="AA42" s="75"/>
     </row>
@@ -8536,9 +8491,7 @@
       <c r="V44" s="74"/>
       <c r="W44" s="74"/>
       <c r="X44" s="75"/>
-      <c r="Y44" s="88" t="s">
-        <v>101</v>
-      </c>
+      <c r="Y44" s="88"/>
       <c r="Z44" s="74"/>
       <c r="AA44" s="75"/>
     </row>
@@ -37611,33 +37564,33 @@
       <c r="K7" s="74"/>
       <c r="L7" s="74"/>
       <c r="M7" s="74"/>
-      <c r="N7" s="125" t="n">
+      <c r="N7" s="125">
         <f>SUM(N11:O111)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O7" s="75"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="126" t="n">
+      <c r="A8" s="126">
         <f>COUNTA(C11:C111)</f>
-        <v>3.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="127"/>
       <c r="C8" s="128"/>
-      <c r="D8" s="99" t="n">
+      <c r="D8" s="99">
         <f>SUM(D11:E111)</f>
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="E8" s="75"/>
-      <c r="F8" s="26" t="n">
+      <c r="F8" s="26">
         <f t="shared" ref="F8:G8" si="0">SUM(F11:F111)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
-      <c r="G8" s="26" t="n">
+      <c r="G8" s="26">
         <f t="shared" si="0"/>
-        <v>4.4</v>
+        <v>0</v>
       </c>
       <c r="H8" s="130"/>
       <c r="I8" s="146"/>
@@ -37713,16 +37666,12 @@
       <c r="Q10" s="28"/>
     </row>
     <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="8">
         <f>ROW()-10</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>149</v>
-      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
@@ -37739,24 +37688,16 @@
       <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="n">
+      <c r="A12" s="8" t="str">
         <f t="shared" ref="A12:A111" si="1">IF(OR(ISBLANK(C12),ISBLANK(B12)), "", ROW()-10)</f>
-        <v>2.0</v>
+        <v/>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="32" t="n">
-        <v>3.0</v>
-      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="34"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="34" t="n">
-        <v>3.0</v>
-      </c>
+      <c r="G12" s="34"/>
       <c r="H12" s="34"/>
       <c r="I12" s="146"/>
       <c r="J12" s="33"/>
@@ -37769,24 +37710,16 @@
       <c r="Q12" s="35"/>
     </row>
     <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="n">
+      <c r="A13" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>3.0</v>
+        <v/>
       </c>
-      <c r="B13" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="32" t="n">
-        <v>1.6</v>
-      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="34"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="34" t="n">
-        <v>1.4</v>
-      </c>
+      <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="146"/>
       <c r="J13" s="33" t="str">
@@ -55816,33 +55749,33 @@
         <v>125</v>
       </c>
       <c r="C13" s="74"/>
-      <c r="D13" s="8" t="n">
+      <c r="D13" s="8">
         <f>COUNTA(C17:G26)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E13" s="153" t="s">
         <v>126</v>
       </c>
       <c r="F13" s="74"/>
-      <c r="G13" s="41" t="n">
+      <c r="G13" s="41">
         <f>SUM(H17:I26)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H13" s="153" t="s">
         <v>127</v>
       </c>
       <c r="I13" s="74"/>
-      <c r="J13" s="41" t="n">
+      <c r="J13" s="41">
         <f>SUM(J17:K26)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K13" s="153" t="s">
         <v>128</v>
       </c>
       <c r="L13" s="74"/>
-      <c r="M13" s="41" t="n">
+      <c r="M13" s="41">
         <f>SUM(L17:M26)</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N13" s="42"/>
     </row>
@@ -55918,18 +55851,18 @@
       <c r="I17" s="75"/>
       <c r="J17" s="152"/>
       <c r="K17" s="75"/>
-      <c r="L17" s="99" t="n">
+      <c r="L17" s="99">
         <f t="shared" ref="L17:L26" si="0">H17+J17</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M17" s="75"/>
       <c r="N17" s="146"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="146"/>
-      <c r="B18" s="15" t="n">
+      <c r="B18" s="15">
         <f t="shared" ref="B18:B26" si="1">B17+1</f>
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="88"/>
       <c r="D18" s="74"/>
@@ -55940,18 +55873,18 @@
       <c r="I18" s="75"/>
       <c r="J18" s="152"/>
       <c r="K18" s="75"/>
-      <c r="L18" s="99" t="n">
+      <c r="L18" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M18" s="75"/>
       <c r="N18" s="146"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="146"/>
-      <c r="B19" s="15" t="n">
+      <c r="B19" s="15">
         <f t="shared" si="1"/>
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="88"/>
       <c r="D19" s="74"/>
@@ -55962,18 +55895,18 @@
       <c r="I19" s="75"/>
       <c r="J19" s="152"/>
       <c r="K19" s="75"/>
-      <c r="L19" s="99" t="n">
+      <c r="L19" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M19" s="75"/>
       <c r="N19" s="146"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="146"/>
-      <c r="B20" s="15" t="n">
+      <c r="B20" s="15">
         <f t="shared" si="1"/>
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C20" s="88"/>
       <c r="D20" s="74"/>
@@ -55984,18 +55917,18 @@
       <c r="I20" s="75"/>
       <c r="J20" s="152"/>
       <c r="K20" s="75"/>
-      <c r="L20" s="99" t="n">
+      <c r="L20" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M20" s="75"/>
       <c r="N20" s="146"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="146"/>
-      <c r="B21" s="15" t="n">
+      <c r="B21" s="15">
         <f t="shared" si="1"/>
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C21" s="88"/>
       <c r="D21" s="74"/>
@@ -56006,18 +55939,18 @@
       <c r="I21" s="75"/>
       <c r="J21" s="152"/>
       <c r="K21" s="75"/>
-      <c r="L21" s="99" t="n">
+      <c r="L21" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M21" s="75"/>
       <c r="N21" s="146"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="146"/>
-      <c r="B22" s="15" t="n">
+      <c r="B22" s="15">
         <f t="shared" si="1"/>
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C22" s="88"/>
       <c r="D22" s="74"/>
@@ -56028,18 +55961,18 @@
       <c r="I22" s="75"/>
       <c r="J22" s="152"/>
       <c r="K22" s="75"/>
-      <c r="L22" s="99" t="n">
+      <c r="L22" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M22" s="75"/>
       <c r="N22" s="146"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="146"/>
-      <c r="B23" s="15" t="n">
+      <c r="B23" s="15">
         <f t="shared" si="1"/>
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C23" s="88"/>
       <c r="D23" s="74"/>
@@ -56050,18 +55983,18 @@
       <c r="I23" s="75"/>
       <c r="J23" s="152"/>
       <c r="K23" s="75"/>
-      <c r="L23" s="99" t="n">
+      <c r="L23" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M23" s="75"/>
       <c r="N23" s="146"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="146"/>
-      <c r="B24" s="15" t="n">
+      <c r="B24" s="15">
         <f t="shared" si="1"/>
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C24" s="88"/>
       <c r="D24" s="74"/>
@@ -56072,18 +56005,18 @@
       <c r="I24" s="75"/>
       <c r="J24" s="152"/>
       <c r="K24" s="75"/>
-      <c r="L24" s="99" t="n">
+      <c r="L24" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M24" s="75"/>
       <c r="N24" s="146"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="146"/>
-      <c r="B25" s="15" t="n">
+      <c r="B25" s="15">
         <f t="shared" si="1"/>
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C25" s="88"/>
       <c r="D25" s="74"/>
@@ -56094,18 +56027,18 @@
       <c r="I25" s="75"/>
       <c r="J25" s="152"/>
       <c r="K25" s="75"/>
-      <c r="L25" s="99" t="n">
+      <c r="L25" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M25" s="75"/>
       <c r="N25" s="146"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="130"/>
-      <c r="B26" s="15" t="n">
+      <c r="B26" s="15">
         <f t="shared" si="1"/>
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C26" s="88"/>
       <c r="D26" s="74"/>
@@ -56116,9 +56049,9 @@
       <c r="I26" s="75"/>
       <c r="J26" s="152"/>
       <c r="K26" s="75"/>
-      <c r="L26" s="99" t="n">
+      <c r="L26" s="99">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M26" s="75"/>
       <c r="N26" s="130"/>
@@ -57390,9 +57323,9 @@
       </c>
       <c r="K13" s="74"/>
       <c r="L13" s="75"/>
-      <c r="M13" s="45" t="n">
+      <c r="M13" s="45">
         <f>E13-I13</f>
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N13" s="46"/>
     </row>

</xml_diff>

<commit_message>
Updated pom.xml. Added download button to GUI2 and implemented its functionality.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="150">
   <si>
     <r>
       <rPr>
@@ -1205,6 +1205,21 @@
   </si>
   <si>
     <t>editCell test</t>
+  </si>
+  <si>
+    <t>Glenn</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Montepiedra</t>
   </si>
 </sst>
 </file>
@@ -7569,32 +7584,32 @@
       </c>
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="117">
+      <c r="A18" s="117" t="str">
         <f>F24</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="B18" s="75"/>
-      <c r="C18" s="93">
+      <c r="C18" s="93" t="str">
         <f>B24</f>
-        <v>0</v>
+        <v>Glenn</v>
       </c>
       <c r="D18" s="74"/>
       <c r="E18" s="75"/>
-      <c r="F18" s="7">
+      <c r="F18" s="7" t="n">
         <f>Attendance!A8</f>
-        <v>0</v>
+        <v>1.0</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="7" t="n">
         <f>IF(ISBLANK(Attendance!D8), "", Attendance!D8)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="7" t="n">
         <f>IF(ISBLANK(Attendance!F8), "", Attendance!F8)</f>
-        <v>0</v>
+        <v>1.0</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="7" t="n">
         <f>IF(ISBLANK(Attendance!G8), "", Attendance!G8)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="J18" s="8" t="str">
         <f>IF(ISBLANK(G37),"",G37)</f>
@@ -7602,7 +7617,7 @@
       </c>
       <c r="K18" s="8" t="str">
         <f>IF(ISBLANK(G38),"",G38)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="L18" s="8" t="str">
         <f>IF(ISBLANK(G39),"",G39)</f>
@@ -7622,7 +7637,7 @@
       </c>
       <c r="P18" s="8" t="str">
         <f>IF(ISBLANK(G45),"",G45)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="Q18" s="8" t="str">
         <f>IF(ISBLANK(G49), "", G49)</f>
@@ -7646,7 +7661,7 @@
       </c>
       <c r="V18" s="8" t="str">
         <f>IF(ISBLANK(Y41), "", Y41)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="W18" s="8" t="str">
         <f>IF(ISBLANK(Y42), "", Y42)</f>
@@ -7662,7 +7677,7 @@
       </c>
       <c r="Z18" s="8" t="str">
         <f>IF(ISBLANK(Y45), "", Y45)</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AA18" s="9" t="str">
         <f>IF(ISBLANK(Y46), "", Y46)</f>
@@ -7823,13 +7838,17 @@
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="101"/>
       <c r="B24" s="88" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C24" s="74"/>
       <c r="D24" s="75"/>
       <c r="E24" s="98"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
+      <c r="F24" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="H24" s="98"/>
       <c r="I24" s="94" t="s">
         <v>71</v>
@@ -7863,7 +7882,7 @@
       <c r="G25" s="49"/>
       <c r="H25" s="98"/>
       <c r="I25" s="88" t="s">
-        <v>72</v>
+        <v>147</v>
       </c>
       <c r="J25" s="74"/>
       <c r="K25" s="74"/>
@@ -7919,13 +7938,15 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="101"/>
-      <c r="B27" s="88"/>
+      <c r="B27" s="88" t="s">
+        <v>64</v>
+      </c>
       <c r="C27" s="74"/>
       <c r="D27" s="75"/>
       <c r="E27" s="98"/>
-      <c r="F27" s="99">
+      <c r="F27" s="99" t="n">
         <f>'Driving Info'!M13</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G27" s="75"/>
       <c r="H27" s="98"/>
@@ -7993,7 +8014,9 @@
       </c>
       <c r="G29" s="75"/>
       <c r="H29" s="98"/>
-      <c r="I29" s="88"/>
+      <c r="I29" s="88" t="s">
+        <v>147</v>
+      </c>
       <c r="J29" s="74"/>
       <c r="K29" s="74"/>
       <c r="L29" s="74"/>
@@ -8015,13 +8038,15 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="101"/>
-      <c r="B30" s="102"/>
+      <c r="B30" s="102" t="s">
+        <v>146</v>
+      </c>
       <c r="C30" s="74"/>
       <c r="D30" s="75"/>
       <c r="E30" s="98"/>
-      <c r="F30" s="118">
+      <c r="F30" s="118" t="n">
         <f>Fundraising!M13</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G30" s="75"/>
       <c r="H30" s="98"/>
@@ -8273,7 +8298,9 @@
       <c r="D38" s="74"/>
       <c r="E38" s="74"/>
       <c r="F38" s="75"/>
-      <c r="G38" s="15"/>
+      <c r="G38" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="H38" s="113"/>
       <c r="I38" s="114"/>
       <c r="J38" s="115" t="s">
@@ -8392,7 +8419,9 @@
       <c r="V41" s="74"/>
       <c r="W41" s="74"/>
       <c r="X41" s="75"/>
-      <c r="Y41" s="88"/>
+      <c r="Y41" s="88" t="s">
+        <v>101</v>
+      </c>
       <c r="Z41" s="74"/>
       <c r="AA41" s="75"/>
     </row>
@@ -8504,7 +8533,9 @@
       <c r="D45" s="74"/>
       <c r="E45" s="74"/>
       <c r="F45" s="75"/>
-      <c r="G45" s="15"/>
+      <c r="G45" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="H45" s="113"/>
       <c r="I45" s="114"/>
       <c r="J45" s="115" t="s">
@@ -8524,7 +8555,9 @@
       <c r="V45" s="74"/>
       <c r="W45" s="74"/>
       <c r="X45" s="75"/>
-      <c r="Y45" s="88"/>
+      <c r="Y45" s="88" t="s">
+        <v>101</v>
+      </c>
       <c r="Z45" s="74"/>
       <c r="AA45" s="75"/>
     </row>
@@ -37564,33 +37597,33 @@
       <c r="K7" s="74"/>
       <c r="L7" s="74"/>
       <c r="M7" s="74"/>
-      <c r="N7" s="125">
+      <c r="N7" s="125" t="n">
         <f>SUM(N11:O111)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="O7" s="75"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="126">
+      <c r="A8" s="126" t="n">
         <f>COUNTA(C11:C111)</f>
-        <v>0</v>
+        <v>1.0</v>
       </c>
       <c r="B8" s="127"/>
       <c r="C8" s="128"/>
-      <c r="D8" s="99">
+      <c r="D8" s="99" t="n">
         <f>SUM(D11:E111)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E8" s="75"/>
-      <c r="F8" s="26">
+      <c r="F8" s="26" t="n">
         <f t="shared" ref="F8:G8" si="0">SUM(F11:F111)</f>
-        <v>0</v>
+        <v>1.0</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" s="130"/>
       <c r="I8" s="146"/>
@@ -37666,15 +37699,21 @@
       <c r="Q10" s="28"/>
     </row>
     <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="8" t="n">
         <f>ROW()-10</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
+      <c r="B11" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>149</v>
+      </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="F11" s="32" t="n">
+        <v>1.0</v>
+      </c>
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
       <c r="I11" s="146"/>
@@ -55749,33 +55788,33 @@
         <v>125</v>
       </c>
       <c r="C13" s="74"/>
-      <c r="D13" s="8">
+      <c r="D13" s="8" t="n">
         <f>COUNTA(C17:G26)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E13" s="153" t="s">
         <v>126</v>
       </c>
       <c r="F13" s="74"/>
-      <c r="G13" s="41">
+      <c r="G13" s="41" t="n">
         <f>SUM(H17:I26)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H13" s="153" t="s">
         <v>127</v>
       </c>
       <c r="I13" s="74"/>
-      <c r="J13" s="41">
+      <c r="J13" s="41" t="n">
         <f>SUM(J17:K26)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="K13" s="153" t="s">
         <v>128</v>
       </c>
       <c r="L13" s="74"/>
-      <c r="M13" s="41">
+      <c r="M13" s="41" t="n">
         <f>SUM(L17:M26)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="N13" s="42"/>
     </row>
@@ -55851,18 +55890,18 @@
       <c r="I17" s="75"/>
       <c r="J17" s="152"/>
       <c r="K17" s="75"/>
-      <c r="L17" s="99">
+      <c r="L17" s="99" t="n">
         <f t="shared" ref="L17:L26" si="0">H17+J17</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M17" s="75"/>
       <c r="N17" s="146"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="146"/>
-      <c r="B18" s="15">
+      <c r="B18" s="15" t="n">
         <f t="shared" ref="B18:B26" si="1">B17+1</f>
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="C18" s="88"/>
       <c r="D18" s="74"/>
@@ -55873,18 +55912,18 @@
       <c r="I18" s="75"/>
       <c r="J18" s="152"/>
       <c r="K18" s="75"/>
-      <c r="L18" s="99">
+      <c r="L18" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M18" s="75"/>
       <c r="N18" s="146"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="146"/>
-      <c r="B19" s="15">
+      <c r="B19" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="C19" s="88"/>
       <c r="D19" s="74"/>
@@ -55895,18 +55934,18 @@
       <c r="I19" s="75"/>
       <c r="J19" s="152"/>
       <c r="K19" s="75"/>
-      <c r="L19" s="99">
+      <c r="L19" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M19" s="75"/>
       <c r="N19" s="146"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="146"/>
-      <c r="B20" s="15">
+      <c r="B20" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="C20" s="88"/>
       <c r="D20" s="74"/>
@@ -55917,18 +55956,18 @@
       <c r="I20" s="75"/>
       <c r="J20" s="152"/>
       <c r="K20" s="75"/>
-      <c r="L20" s="99">
+      <c r="L20" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M20" s="75"/>
       <c r="N20" s="146"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="146"/>
-      <c r="B21" s="15">
+      <c r="B21" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.0</v>
       </c>
       <c r="C21" s="88"/>
       <c r="D21" s="74"/>
@@ -55939,18 +55978,18 @@
       <c r="I21" s="75"/>
       <c r="J21" s="152"/>
       <c r="K21" s="75"/>
-      <c r="L21" s="99">
+      <c r="L21" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M21" s="75"/>
       <c r="N21" s="146"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="146"/>
-      <c r="B22" s="15">
+      <c r="B22" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>6.0</v>
       </c>
       <c r="C22" s="88"/>
       <c r="D22" s="74"/>
@@ -55961,18 +56000,18 @@
       <c r="I22" s="75"/>
       <c r="J22" s="152"/>
       <c r="K22" s="75"/>
-      <c r="L22" s="99">
+      <c r="L22" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M22" s="75"/>
       <c r="N22" s="146"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="146"/>
-      <c r="B23" s="15">
+      <c r="B23" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>7.0</v>
       </c>
       <c r="C23" s="88"/>
       <c r="D23" s="74"/>
@@ -55983,18 +56022,18 @@
       <c r="I23" s="75"/>
       <c r="J23" s="152"/>
       <c r="K23" s="75"/>
-      <c r="L23" s="99">
+      <c r="L23" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M23" s="75"/>
       <c r="N23" s="146"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="146"/>
-      <c r="B24" s="15">
+      <c r="B24" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="C24" s="88"/>
       <c r="D24" s="74"/>
@@ -56005,18 +56044,18 @@
       <c r="I24" s="75"/>
       <c r="J24" s="152"/>
       <c r="K24" s="75"/>
-      <c r="L24" s="99">
+      <c r="L24" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M24" s="75"/>
       <c r="N24" s="146"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="146"/>
-      <c r="B25" s="15">
+      <c r="B25" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>9.0</v>
       </c>
       <c r="C25" s="88"/>
       <c r="D25" s="74"/>
@@ -56027,18 +56066,18 @@
       <c r="I25" s="75"/>
       <c r="J25" s="152"/>
       <c r="K25" s="75"/>
-      <c r="L25" s="99">
+      <c r="L25" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M25" s="75"/>
       <c r="N25" s="146"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="130"/>
-      <c r="B26" s="15">
+      <c r="B26" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>10.0</v>
       </c>
       <c r="C26" s="88"/>
       <c r="D26" s="74"/>
@@ -56049,9 +56088,9 @@
       <c r="I26" s="75"/>
       <c r="J26" s="152"/>
       <c r="K26" s="75"/>
-      <c r="L26" s="99">
+      <c r="L26" s="99" t="n">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M26" s="75"/>
       <c r="N26" s="130"/>
@@ -57323,9 +57362,9 @@
       </c>
       <c r="K13" s="74"/>
       <c r="L13" s="75"/>
-      <c r="M13" s="45">
+      <c r="M13" s="45" t="n">
         <f>E13-I13</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="N13" s="46"/>
     </row>

</xml_diff>